<commit_message>
added further analysis points
</commit_message>
<xml_diff>
--- a/0-20000.xlsx
+++ b/0-20000.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="70">
   <si>
     <t>CVR</t>
   </si>
@@ -31,6 +31,12 @@
     <t>Opsagt dato:</t>
   </si>
   <si>
+    <t>Årsag</t>
+  </si>
+  <si>
+    <t>Ny leverandør</t>
+  </si>
+  <si>
     <t>TCV_range</t>
   </si>
   <si>
@@ -182,6 +188,39 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Pris</t>
+  </si>
+  <si>
+    <t>Bruger ikke produktet</t>
+  </si>
+  <si>
+    <t>Anden årsag (angiv hvilken i bemærkninger)</t>
+  </si>
+  <si>
+    <t>Strategisk beslutning</t>
+  </si>
+  <si>
+    <t>Fusionerer med anden virksomhed</t>
+  </si>
+  <si>
+    <t>Ikke oplyst</t>
+  </si>
+  <si>
+    <t>Virksomheden lukker</t>
+  </si>
+  <si>
+    <t>Utilfredshed (Service - uddyb i bemærkninger)</t>
+  </si>
+  <si>
+    <t>Danløn</t>
+  </si>
+  <si>
+    <t>Lessor</t>
+  </si>
+  <si>
+    <t>DataLøn</t>
   </si>
   <si>
     <t>0-20000</t>
@@ -546,13 +585,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,10 +610,16 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>2021</v>
@@ -583,18 +628,21 @@
         <v>13053.78</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E2" s="2">
         <v>44224</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>58</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>2021</v>
@@ -603,18 +651,21 @@
         <v>15000</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E3" s="2">
         <v>44267</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>59</v>
+      </c>
+      <c r="H3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>2021</v>
@@ -623,18 +674,24 @@
         <v>17060.16</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E4" s="2">
         <v>44279</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>60</v>
+      </c>
+      <c r="G4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>2021</v>
@@ -643,18 +700,24 @@
         <v>14114.21</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E5" s="2">
         <v>44293</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>60</v>
+      </c>
+      <c r="G5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>2021</v>
@@ -663,18 +726,21 @@
         <v>12344.44</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2">
         <v>44285</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>61</v>
+      </c>
+      <c r="H6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>2021</v>
@@ -683,18 +749,21 @@
         <v>15000</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E7" s="2">
         <v>44300</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>59</v>
+      </c>
+      <c r="H7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>2021</v>
@@ -703,18 +772,21 @@
         <v>15563.96</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E8" s="2">
         <v>44306</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>62</v>
+      </c>
+      <c r="H8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>2021</v>
@@ -723,18 +795,21 @@
         <v>15511.36</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E9" s="2">
         <v>44326</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>59</v>
+      </c>
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>2021</v>
@@ -743,18 +818,21 @@
         <v>19589.49</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E10" s="2">
         <v>44336</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>62</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>2021</v>
@@ -763,18 +841,21 @@
         <v>18049.5</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E11" s="2">
         <v>44410</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>63</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>2021</v>
@@ -783,18 +864,21 @@
         <v>17258.07</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E12" s="2">
         <v>44489</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>64</v>
+      </c>
+      <c r="H12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>2021</v>
@@ -803,18 +887,21 @@
         <v>11524</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E13" s="2">
         <v>44503</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>59</v>
+      </c>
+      <c r="H13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>2021</v>
@@ -823,18 +910,21 @@
         <v>18103.47</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E14" s="2">
         <v>44523</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>63</v>
+      </c>
+      <c r="H14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B15">
         <v>2021</v>
@@ -843,18 +933,21 @@
         <v>18120</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E15" s="2">
         <v>44498</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>65</v>
+      </c>
+      <c r="H15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>2022</v>
@@ -863,18 +956,21 @@
         <v>16357.92</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E16" s="2">
         <v>44589</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>63</v>
+      </c>
+      <c r="H16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>2022</v>
@@ -883,18 +979,21 @@
         <v>18108</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E17" s="2">
         <v>44594</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>63</v>
+      </c>
+      <c r="H17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <v>2022</v>
@@ -903,18 +1002,21 @@
         <v>12087</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E18" s="2">
         <v>44620</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>63</v>
+      </c>
+      <c r="H18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B19">
         <v>2022</v>
@@ -923,18 +1025,21 @@
         <v>4467</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E19" s="2">
         <v>44634</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>60</v>
+      </c>
+      <c r="H19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B20">
         <v>2022</v>
@@ -943,18 +1048,21 @@
         <v>19712.96</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E20" s="2">
         <v>44649</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>60</v>
+      </c>
+      <c r="H20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B21">
         <v>2022</v>
@@ -963,18 +1071,21 @@
         <v>5520</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E21" s="2">
         <v>44652</v>
       </c>
       <c r="F21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>60</v>
+      </c>
+      <c r="H21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B22">
         <v>2022</v>
@@ -983,18 +1094,24 @@
         <v>15000</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E22" s="2">
         <v>44655</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>59</v>
+      </c>
+      <c r="G22" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B23">
         <v>2022</v>
@@ -1003,18 +1120,21 @@
         <v>5500</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E23" s="2">
         <v>44672</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>60</v>
+      </c>
+      <c r="H23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B24">
         <v>2022</v>
@@ -1023,18 +1143,21 @@
         <v>15000</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E24" s="2">
         <v>44719</v>
       </c>
       <c r="F24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>61</v>
+      </c>
+      <c r="H24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B25">
         <v>2022</v>
@@ -1043,18 +1166,21 @@
         <v>12000</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E25" s="2">
         <v>44775</v>
       </c>
       <c r="F25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>63</v>
+      </c>
+      <c r="H25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B26">
         <v>2022</v>
@@ -1063,18 +1189,21 @@
         <v>18449</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E26" s="2">
         <v>44820</v>
       </c>
       <c r="F26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>64</v>
+      </c>
+      <c r="H26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B27">
         <v>2022</v>
@@ -1083,18 +1212,21 @@
         <v>9000</v>
       </c>
       <c r="D27" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E27" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>60</v>
+      </c>
+      <c r="H27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B28">
         <v>2022</v>
@@ -1103,18 +1235,21 @@
         <v>15360</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E28" s="2">
         <v>44852</v>
       </c>
       <c r="F28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>60</v>
+      </c>
+      <c r="H28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B29">
         <v>2022</v>
@@ -1123,18 +1258,21 @@
         <v>17098</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E29" s="2">
         <v>44861</v>
       </c>
       <c r="F29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>61</v>
+      </c>
+      <c r="H29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B30">
         <v>2022</v>
@@ -1143,18 +1281,21 @@
         <v>16796</v>
       </c>
       <c r="D30" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E30" s="2">
         <v>44865</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>64</v>
+      </c>
+      <c r="H30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B31">
         <v>2022</v>
@@ -1163,18 +1304,21 @@
         <v>15000</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E31" s="2">
         <v>44837</v>
       </c>
       <c r="F31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>61</v>
+      </c>
+      <c r="H31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B32">
         <v>2022</v>
@@ -1183,18 +1327,21 @@
         <v>3432</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E32" s="2">
         <v>44895</v>
       </c>
       <c r="F32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>65</v>
+      </c>
+      <c r="H32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B33">
         <v>2022</v>
@@ -1203,18 +1350,21 @@
         <v>6072</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E33" s="2">
         <v>44915</v>
       </c>
       <c r="F33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>63</v>
+      </c>
+      <c r="H33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B34">
         <v>2023</v>
@@ -1223,18 +1373,21 @@
         <v>4512</v>
       </c>
       <c r="D34" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E34" s="2">
         <v>44928</v>
       </c>
       <c r="F34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>63</v>
+      </c>
+      <c r="H34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B35">
         <v>2023</v>
@@ -1243,18 +1396,21 @@
         <v>6137</v>
       </c>
       <c r="D35" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E35" s="2">
         <v>44951</v>
       </c>
       <c r="F35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>63</v>
+      </c>
+      <c r="H35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B36">
         <v>2023</v>
@@ -1263,18 +1419,21 @@
         <v>6564</v>
       </c>
       <c r="D36" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E36" s="2">
         <v>44979</v>
       </c>
       <c r="F36" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>59</v>
+      </c>
+      <c r="H36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B37">
         <v>2023</v>
@@ -1283,18 +1442,21 @@
         <v>4513</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E37" s="2">
         <v>45027</v>
       </c>
       <c r="F37" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>59</v>
+      </c>
+      <c r="H37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B38">
         <v>2023</v>
@@ -1303,18 +1465,21 @@
         <v>18378</v>
       </c>
       <c r="D38" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E38" s="2">
         <v>45048</v>
       </c>
       <c r="F38" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>59</v>
+      </c>
+      <c r="H38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B39">
         <v>2023</v>
@@ -1323,13 +1488,16 @@
         <v>6277</v>
       </c>
       <c r="D39" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E39" s="2">
         <v>45048</v>
       </c>
       <c r="F39" t="s">
-        <v>56</v>
+        <v>63</v>
+      </c>
+      <c r="H39" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated entire analysis with newest numbers from 7th October 2024
</commit_message>
<xml_diff>
--- a/0-20000.xlsx
+++ b/0-20000.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="91">
   <si>
     <t>CVR</t>
   </si>
@@ -160,6 +160,21 @@
     <t>30715993</t>
   </si>
   <si>
+    <t>56216316</t>
+  </si>
+  <si>
+    <t>26092515</t>
+  </si>
+  <si>
+    <t>18912236</t>
+  </si>
+  <si>
+    <t>32551335</t>
+  </si>
+  <si>
+    <t>66590119</t>
+  </si>
+  <si>
     <t>Visma Løn og HR</t>
   </si>
   <si>
@@ -263,6 +278,12 @@
   </si>
   <si>
     <t>2023Q2</t>
+  </si>
+  <si>
+    <t>2024Q1</t>
+  </si>
+  <si>
+    <t>2024Q2</t>
   </si>
   <si>
     <t>0-20000</t>
@@ -627,7 +648,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -673,19 +694,19 @@
         <v>13053.78</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E2" s="2">
         <v>44224</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="H2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -699,19 +720,19 @@
         <v>15000</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E3" s="2">
         <v>44267</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I3" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -725,22 +746,22 @@
         <v>17060.16</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E4" s="2">
         <v>44279</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -754,22 +775,22 @@
         <v>14114.21</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E5" s="2">
         <v>44293</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="I5" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -783,19 +804,19 @@
         <v>12344.44</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E6" s="2">
         <v>44285</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I6" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -809,19 +830,19 @@
         <v>15000</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E7" s="2">
         <v>44300</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="H7" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="I7" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -835,19 +856,19 @@
         <v>15563.96</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E8" s="2">
         <v>44306</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H8" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="I8" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -861,19 +882,19 @@
         <v>15511.36</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E9" s="2">
         <v>44326</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="H9" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="I9" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -887,19 +908,19 @@
         <v>19589.49</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E10" s="2">
         <v>44336</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H10" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="I10" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -913,19 +934,19 @@
         <v>18049.5</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E11" s="2">
         <v>44410</v>
       </c>
       <c r="F11" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H11" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I11" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -939,19 +960,19 @@
         <v>17258.07</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E12" s="2">
         <v>44489</v>
       </c>
       <c r="F12" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="H12" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="I12" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -965,19 +986,19 @@
         <v>11524</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E13" s="2">
         <v>44503</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="H13" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -991,19 +1012,19 @@
         <v>18103.47</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E14" s="2">
         <v>44523</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1017,19 +1038,19 @@
         <v>18120</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E15" s="2">
         <v>44498</v>
       </c>
       <c r="F15" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="H15" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="I15" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1043,19 +1064,19 @@
         <v>16357.92</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E16" s="2">
         <v>44589</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H16" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I16" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1069,19 +1090,19 @@
         <v>18108</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E17" s="2">
         <v>44594</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H17" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I17" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1095,19 +1116,19 @@
         <v>12087</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E18" s="2">
         <v>44620</v>
       </c>
       <c r="F18" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H18" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I18" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1121,19 +1142,19 @@
         <v>4467</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E19" s="2">
         <v>44634</v>
       </c>
       <c r="F19" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H19" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I19" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1147,19 +1168,19 @@
         <v>19712.96</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E20" s="2">
         <v>44649</v>
       </c>
       <c r="F20" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H20" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1173,19 +1194,19 @@
         <v>5520</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E21" s="2">
         <v>44652</v>
       </c>
       <c r="F21" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H21" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I21" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1199,22 +1220,22 @@
         <v>15000</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E22" s="2">
         <v>44655</v>
       </c>
       <c r="F22" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="G22" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H22" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I22" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1228,19 +1249,19 @@
         <v>5500</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E23" s="2">
         <v>44672</v>
       </c>
       <c r="F23" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H23" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I23" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1254,19 +1275,19 @@
         <v>15000</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E24" s="2">
         <v>44719</v>
       </c>
       <c r="F24" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H24" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I24" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1280,19 +1301,19 @@
         <v>12000</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E25" s="2">
         <v>44775</v>
       </c>
       <c r="F25" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H25" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="I25" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1306,19 +1327,19 @@
         <v>18449</v>
       </c>
       <c r="D26" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E26" s="2">
         <v>44820</v>
       </c>
       <c r="F26" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="H26" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="I26" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1332,13 +1353,13 @@
         <v>9000</v>
       </c>
       <c r="D27" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F27" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I27" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1352,19 +1373,19 @@
         <v>15360</v>
       </c>
       <c r="D28" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E28" s="2">
         <v>44852</v>
       </c>
       <c r="F28" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H28" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="I28" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1378,19 +1399,19 @@
         <v>17098</v>
       </c>
       <c r="D29" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E29" s="2">
         <v>44861</v>
       </c>
       <c r="F29" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H29" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="I29" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1404,19 +1425,19 @@
         <v>16796</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E30" s="2">
         <v>44865</v>
       </c>
       <c r="F30" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="H30" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="I30" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1430,19 +1451,19 @@
         <v>15000</v>
       </c>
       <c r="D31" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E31" s="2">
         <v>44837</v>
       </c>
       <c r="F31" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H31" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="I31" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1456,19 +1477,19 @@
         <v>3432</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E32" s="2">
         <v>44895</v>
       </c>
       <c r="F32" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="H32" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="I32" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1482,19 +1503,19 @@
         <v>6072</v>
       </c>
       <c r="D33" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E33" s="2">
         <v>44915</v>
       </c>
       <c r="F33" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H33" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="I33" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1508,16 +1529,16 @@
         <v>4512</v>
       </c>
       <c r="D34" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E34" s="2">
         <v>44928</v>
       </c>
       <c r="H34" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I34" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1531,16 +1552,16 @@
         <v>6137</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E35" s="2">
         <v>44951</v>
       </c>
       <c r="H35" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I35" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1554,16 +1575,16 @@
         <v>6564</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E36" s="2">
         <v>44979</v>
       </c>
       <c r="H36" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I36" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1577,16 +1598,16 @@
         <v>4513</v>
       </c>
       <c r="D37" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E37" s="2">
         <v>45027</v>
       </c>
       <c r="H37" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I37" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1600,16 +1621,16 @@
         <v>18378</v>
       </c>
       <c r="D38" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E38" s="2">
         <v>45048</v>
       </c>
       <c r="H38" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I38" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1623,16 +1644,16 @@
         <v>6277</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E39" s="2">
         <v>45048</v>
       </c>
       <c r="H39" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I39" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1646,16 +1667,16 @@
         <v>19530</v>
       </c>
       <c r="D40" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E40" s="2">
         <v>45083</v>
       </c>
       <c r="H40" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I40" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1669,19 +1690,137 @@
         <v>6371</v>
       </c>
       <c r="D41" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E41" s="2">
         <v>45106</v>
       </c>
       <c r="G41" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H41" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I41" t="s">
-        <v>83</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42">
+        <v>2024</v>
+      </c>
+      <c r="C42">
+        <v>16783.1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" s="2">
+        <v>45372</v>
+      </c>
+      <c r="G42" t="s">
+        <v>74</v>
+      </c>
+      <c r="H42" t="s">
+        <v>88</v>
+      </c>
+      <c r="I42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43">
+        <v>2024</v>
+      </c>
+      <c r="C43">
+        <v>18300</v>
+      </c>
+      <c r="D43" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43" s="2">
+        <v>45400</v>
+      </c>
+      <c r="H43" t="s">
+        <v>89</v>
+      </c>
+      <c r="I43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44">
+        <v>2024</v>
+      </c>
+      <c r="C44">
+        <v>19350</v>
+      </c>
+      <c r="D44" t="s">
+        <v>55</v>
+      </c>
+      <c r="E44" s="2">
+        <v>45436</v>
+      </c>
+      <c r="H44" t="s">
+        <v>89</v>
+      </c>
+      <c r="I44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45">
+        <v>2024</v>
+      </c>
+      <c r="C45">
+        <v>6708.12</v>
+      </c>
+      <c r="D45" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" s="2">
+        <v>45378</v>
+      </c>
+      <c r="H45" t="s">
+        <v>88</v>
+      </c>
+      <c r="I45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46">
+        <v>2024</v>
+      </c>
+      <c r="C46">
+        <v>5000</v>
+      </c>
+      <c r="D46" t="s">
+        <v>58</v>
+      </c>
+      <c r="E46" s="2">
+        <v>45457</v>
+      </c>
+      <c r="H46" t="s">
+        <v>89</v>
+      </c>
+      <c r="I46" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>